<commit_message>
Add LEDs for Power and status indication, generate new outputs with these changes
</commit_message>
<xml_diff>
--- a/Default Configuration/Outputs/BOM/BOM_PartType-REFLOW_CONTROLLER_A01.xlsx
+++ b/Default Configuration/Outputs/BOM/BOM_PartType-REFLOW_CONTROLLER_A01.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1261B0B8-4F79-424F-8816-165CA3117276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8767C13-DF8C-4CB0-95A7-62E1A3F63E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{A4C2BBA4-2374-48A8-94B5-F3AB202B596D}"/>
+    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{932B38E3-3D18-46AB-ACD2-4D8CC5C65C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-REFLOW_CONTROLLER_" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="249">
   <si>
     <t>Designator</t>
   </si>
@@ -415,6 +415,45 @@
     <t>C2935898</t>
   </si>
   <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>20mA 54mcd -55?~+85? 631nm Red 130° 75mW 2V 0603 Light Emitting Diodes (LED) ROHS</t>
+  </si>
+  <si>
+    <t>Lite-On</t>
+  </si>
+  <si>
+    <t>LTST-C191KRKT</t>
+  </si>
+  <si>
+    <t>0.014</t>
+  </si>
+  <si>
+    <t>0.011</t>
+  </si>
+  <si>
+    <t>C125099</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>SMD5050 RGB LEDs ROHS</t>
+  </si>
+  <si>
+    <t>HONGLITRONIC</t>
+  </si>
+  <si>
+    <t>HL-AF-5060H248BS36FU76GC-S1-THL</t>
+  </si>
+  <si>
+    <t>0.0325</t>
+  </si>
+  <si>
+    <t>C2683773</t>
+  </si>
+  <si>
     <t>Q1, Q2, Q3</t>
   </si>
   <si>
@@ -472,7 +511,7 @@
     <t>C22548</t>
   </si>
   <si>
-    <t>R4, R12</t>
+    <t>R4, R12, R27, R29</t>
   </si>
   <si>
     <t>100mW Thick Film Resistors 75V ±100ppm/? ±1% 100O 0603 Chip Resistor - Surface Mount ROHS</t>
@@ -569,6 +608,18 @@
   </si>
   <si>
     <t>C163417</t>
+  </si>
+  <si>
+    <t>R28, R30</t>
+  </si>
+  <si>
+    <t>100mW Thick Film Resistors 75V ±100ppm/? ±1% 30O 0603 Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>RC0603FR-0730RL</t>
+  </si>
+  <si>
+    <t>C128060</t>
   </si>
   <si>
     <t>RV1</t>
@@ -1107,8 +1158,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC73B7C-07F0-419F-98CD-08129606E23D}">
-  <dimension ref="A1:I37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F165C0BF-3CB6-412C-A1AE-7BD4F5140565}">
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1674,48 +1725,48 @@
         <v>128</v>
       </c>
       <c r="B20" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>129</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>139</v>
@@ -1732,13 +1783,13 @@
         <v>141</v>
       </c>
       <c r="B22" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>142</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>136</v>
+        <v>58</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>143</v>
@@ -1767,428 +1818,515 @@
         <v>148</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B24" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B25" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B26" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B27" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B31" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="F32" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="H33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B34" s="3">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="H34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="G35" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="H36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>231</v>
+      <c r="D40" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>